<commit_message>
Resubmitting updates after undoing commits due to large file 21/03/16
</commit_message>
<xml_diff>
--- a/Results/GeneExpression/RNA-Seq/read1array.xlsx
+++ b/Results/GeneExpression/RNA-Seq/read1array.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30400" yWindow="1300" windowWidth="25120" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25660" windowHeight="14180" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Petrucelli" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="read1array.txt" sheetId="3" r:id="rId3"/>
+    <sheet name="Ravits" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="233">
   <si>
     <t>Tissue</t>
   </si>
@@ -462,13 +463,271 @@
   </si>
   <si>
     <t>ftp://ftp.sra.ebi.ac.uk/vol1/fastq/SRR192/001/SRR1927071/SRR1927071_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>Sp.Chord</t>
+  </si>
+  <si>
+    <t>GSM1977027</t>
+  </si>
+  <si>
+    <t>GSM1977028</t>
+  </si>
+  <si>
+    <t>GSM1977029</t>
+  </si>
+  <si>
+    <t>GSM1977030</t>
+  </si>
+  <si>
+    <t>GSM1977031</t>
+  </si>
+  <si>
+    <t>GSM1977032</t>
+  </si>
+  <si>
+    <t>GSM1977033</t>
+  </si>
+  <si>
+    <t>GSM1977034</t>
+  </si>
+  <si>
+    <t>GSM1977035</t>
+  </si>
+  <si>
+    <t>GSM1977036</t>
+  </si>
+  <si>
+    <t>GSM1977037</t>
+  </si>
+  <si>
+    <t>GSM1977038</t>
+  </si>
+  <si>
+    <t>GSM1977039</t>
+  </si>
+  <si>
+    <t>GSM1977040</t>
+  </si>
+  <si>
+    <t>GSM1977041</t>
+  </si>
+  <si>
+    <t>GSM1977042</t>
+  </si>
+  <si>
+    <t>GSM1977043</t>
+  </si>
+  <si>
+    <t>GSM1977044</t>
+  </si>
+  <si>
+    <t>GSM1977045</t>
+  </si>
+  <si>
+    <t>GSM1977046</t>
+  </si>
+  <si>
+    <t>GSM1977047</t>
+  </si>
+  <si>
+    <t>SRX1494374</t>
+  </si>
+  <si>
+    <t>SRX1494375</t>
+  </si>
+  <si>
+    <t>SRX1494376</t>
+  </si>
+  <si>
+    <t>SRX1494377</t>
+  </si>
+  <si>
+    <t>SRX1494378</t>
+  </si>
+  <si>
+    <t>SRX1494379</t>
+  </si>
+  <si>
+    <t>SRX1494380</t>
+  </si>
+  <si>
+    <t>SRX1494381</t>
+  </si>
+  <si>
+    <t>SRX1494382</t>
+  </si>
+  <si>
+    <t>SRX1494383</t>
+  </si>
+  <si>
+    <t>SRX1494384</t>
+  </si>
+  <si>
+    <t>SRX1494385</t>
+  </si>
+  <si>
+    <t>SRX1494386</t>
+  </si>
+  <si>
+    <t>SRX1494387</t>
+  </si>
+  <si>
+    <t>SRX1494388</t>
+  </si>
+  <si>
+    <t>SRX1494389</t>
+  </si>
+  <si>
+    <t>SRX1494390</t>
+  </si>
+  <si>
+    <t>SRX1494391</t>
+  </si>
+  <si>
+    <t>SRX1494392</t>
+  </si>
+  <si>
+    <t>SRX1494393</t>
+  </si>
+  <si>
+    <t>SRX1494394</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>SRR3038253</t>
+  </si>
+  <si>
+    <t>SRR3038254</t>
+  </si>
+  <si>
+    <t>SRR3038255</t>
+  </si>
+  <si>
+    <t>SRR3038256</t>
+  </si>
+  <si>
+    <t>SRR3038257</t>
+  </si>
+  <si>
+    <t>SRR3038258</t>
+  </si>
+  <si>
+    <t>SRR3038259</t>
+  </si>
+  <si>
+    <t>SRR3038260</t>
+  </si>
+  <si>
+    <t>SRR3038261</t>
+  </si>
+  <si>
+    <t>SRR3038262</t>
+  </si>
+  <si>
+    <t>SRR3038263</t>
+  </si>
+  <si>
+    <t>SRR3038264</t>
+  </si>
+  <si>
+    <t>SRR3038265</t>
+  </si>
+  <si>
+    <t>SRR3038266</t>
+  </si>
+  <si>
+    <t>SRR3038267</t>
+  </si>
+  <si>
+    <t>SRR3038268</t>
+  </si>
+  <si>
+    <t>SRR3038269</t>
+  </si>
+  <si>
+    <t>SRR3038270</t>
+  </si>
+  <si>
+    <t>SRR3038271</t>
+  </si>
+  <si>
+    <t>SRR3038272</t>
+  </si>
+  <si>
+    <t>SRR3038273</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038253/SRR3038253.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038254/SRR3038254.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038255/SRR3038255.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038256/SRR3038256.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038257/SRR3038257.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038258/SRR3038258.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038259/SRR3038259.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038260/SRR3038260.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038261/SRR3038261.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038262/SRR3038262.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038263/SRR3038263.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038264/SRR3038264.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038265/SRR3038265.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038266/SRR3038266.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038267/SRR3038267.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038268/SRR3038268.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038269/SRR3038269.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038270/SRR3038270.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038271/SRR3038271.sra</t>
+  </si>
+  <si>
+    <t>ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038273/SRR3038273.sra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp://ftp-trace.ncbi.nlm.nih.gov/sra/sra-instant/reads/ByStudy/sra/SRP%2FSRP067%2FSRP067645/SRR3038272/SRR3038272.sra </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -488,6 +747,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -528,7 +795,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -585,6 +852,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,7 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -666,6 +942,15 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -997,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1500,7 +1785,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1916,7 +2201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -2049,4 +2334,536 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="107.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="2">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="2">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="2">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="2">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="2">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="2">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="2">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" s="3">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="3">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="3">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="3">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="3">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="3">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="3">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="3">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" s="3">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="3">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F20" s="3">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F21" s="3">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F22" s="3">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>